<commit_message>
Excel OK + casi sinonimos
</commit_message>
<xml_diff>
--- a/excels/preguntasBase.xlsx
+++ b/excels/preguntasBase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manel\source\repos\YouMakeTheQuestions\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1B07A2-FD1F-4320-9360-2FED600285B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0674529B-7995-41E0-A08D-5A7D2CBA97D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{404A9444-1DB9-49DB-B291-282F4B54CC07}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Es real</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>Es listo</t>
+  </si>
+  <si>
+    <t>Tiene el pelo rubio</t>
   </si>
 </sst>
 </file>
@@ -318,8 +321,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,448 +640,711 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0498C050-0B9A-4589-B44B-755EF6AB0B06}">
-  <dimension ref="A1:A86"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="50.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="50.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>2</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>2</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>2</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>2</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>2</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>2</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>3</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="C31" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>2</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>2</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>2</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>2</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>2</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>2</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>2</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>2</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>2</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>2</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>2</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>2</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>2</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>2</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>2</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>2</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>2</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>2</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>2</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>2</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>2</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>2</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>2</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>2</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>2</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>2</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>2</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>2</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>2</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>2</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>2</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>2</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>2</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>2</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>2</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>2</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>2</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>2</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>2</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>2</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>2</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>2</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>2</v>
+      </c>
+      <c r="B75" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>2</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>2</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>2</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>2</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>2</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>2</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>2</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>2</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>2</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>2</v>
+      </c>
+      <c r="B85" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>2</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>85</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>